<commit_message>
[Update] Implement all questions and relevant functions
</commit_message>
<xml_diff>
--- a/quiz_relevant.xlsx
+++ b/quiz_relevant.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Sapient_backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Sapient\Energy-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3E53F9-9CE0-4F84-8E82-822D93F1A763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA456B6-1AD5-4167-91B7-9D9187D6F1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Questions</t>
   </si>
@@ -70,6 +70,114 @@
   </si>
   <si>
     <t>Return energy consumption by month for [total building]</t>
+  </si>
+  <si>
+    <t>How do I make my building more efficient?</t>
+  </si>
+  <si>
+    <t>How do I make lighting more efficient?</t>
+  </si>
+  <si>
+    <t>Is my building efficient?</t>
+  </si>
+  <si>
+    <t>How can I reduce my carbon footprint?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Try to help answer the question or ask for more specifics. User can be more green by reducing energy usage. they can try inspecting high energy equipment usage and usage outside of operating hours can be helpful.</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Common areas to improve or inspect are energy usage outside of operating hours, end use categories and equipment energy health.</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data.</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Buildings can always be more efficient, sometimes through investment and sometimes through better energy and equipment management.</t>
+  </si>
+  <si>
+    <t>How does September compare to March?</t>
+  </si>
+  <si>
+    <t>Return magnitude of change in energy consumption for [a specific end use category]</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked how two different months compare, ask for specifics of what to compare. Is the user asking for total consumption, equipment, end use category or etc?</t>
+  </si>
+  <si>
+    <t>Why did my energy consumption increase?</t>
+  </si>
+  <si>
+    <t>Return contribution of change to total building energy consumption broken down by [end-use category]</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked if usage has increased without a timeframe. Ask for the specific timeframe.</t>
+  </si>
+  <si>
+    <t>Where should I focus my time today?</t>
+  </si>
+  <si>
+    <t>What are the lowest cost ways to reduce energy consumption in my building?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Inspecting afterhours consuption is a cost effective way to manage energy usage.</t>
+  </si>
+  <si>
+    <t>What lighting circuits are left on during after hours when they shouldn’t be?</t>
+  </si>
+  <si>
+    <t>Return aggregated after hours energy consumption for a specific end use category (and % of total of end use category)</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a specific question which you can not answer. You have no way of assigning what lighting is required to be used during after hours. You should suggest the user reviewing after hour usage in the end category: Lighting.</t>
+  </si>
+  <si>
+    <t>What are the top ten contributors to energy consumption during non-business hours?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Try to help answer the question. Inspecting high energy equipment usage and usage outside of operating hours can be helpful.</t>
+  </si>
+  <si>
+    <t>Which areas of my building tend to consume the most energy in after hours periods?</t>
+  </si>
+  <si>
+    <t>Which plug receptacle circuits are showing the most energy use after hours?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Try to help answer the question. Inspecting high energy plug receptacle circuits usage and usage outside of operating hours can be helpful.</t>
+  </si>
+  <si>
+    <t>What is most contributing to changes in energy consumption patterns this week versus last week?</t>
+  </si>
+  <si>
+    <t>Return contribution of change to total building energy consumption broken down by [specific equipment] (show top 5 in magnitude)</t>
+  </si>
+  <si>
+    <t>What are the top 5 things I should focus on this month to reduce energy consumption in my building?</t>
+  </si>
+  <si>
+    <t>How much of the change in energy consumption of my building is due to changes in weather?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Try to help answer the question. It can be helpful to examine a building's energy usage, which changes with changes in weather.</t>
+  </si>
+  <si>
+    <t>What times of day is energy demand the highest in my building?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked a general question that doesn't require a data. Try to help answer the question. Inspecting changes in energy use over time can be helpful.</t>
+  </si>
+  <si>
+    <t>What are specific measures I can take to reduce peak energy demand in my building?</t>
+  </si>
+  <si>
+    <t>Would installing solar panels reduce the peak demand in my building?</t>
+  </si>
+  <si>
+    <t>How much battery capacity would I need to install to offset the energy demand from the equipment contributing the most to my highest moments of energy demand?</t>
+  </si>
+  <si>
+    <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked how two different weeks compare, ask for specifics of what to compare. Is the user asking for total consumption, equipment, end use category or etc?</t>
   </si>
 </sst>
 </file>
@@ -105,15 +213,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,15 +235,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,17 +547,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="105.28515625" customWidth="1"/>
   </cols>
@@ -487,6 +624,221 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>